<commit_message>
add func updata calJob
</commit_message>
<xml_diff>
--- a/public/tmp/pivottotalwork.xlsx
+++ b/public/tmp/pivottotalwork.xlsx
@@ -53,37 +53,37 @@
     <t>พรชัย</t>
   </si>
   <si>
-    <t>February 2023</t>
-  </si>
-  <si>
-    <t>March 2023</t>
-  </si>
-  <si>
-    <t>April 2023</t>
-  </si>
-  <si>
-    <t>May 2023</t>
-  </si>
-  <si>
-    <t>June 2023</t>
-  </si>
-  <si>
-    <t>July 2023</t>
-  </si>
-  <si>
-    <t>August 2023</t>
-  </si>
-  <si>
-    <t>September 2023</t>
-  </si>
-  <si>
-    <t>October 2023</t>
-  </si>
-  <si>
-    <t>November 2023</t>
-  </si>
-  <si>
-    <t>December 2023</t>
+    <t>February 2024</t>
+  </si>
+  <si>
+    <t>March 2024</t>
+  </si>
+  <si>
+    <t>April 2024</t>
+  </si>
+  <si>
+    <t>May 2024</t>
+  </si>
+  <si>
+    <t>June 2024</t>
+  </si>
+  <si>
+    <t>July 2024</t>
+  </si>
+  <si>
+    <t>August 2024</t>
+  </si>
+  <si>
+    <t>September 2024</t>
+  </si>
+  <si>
+    <t>October 2024</t>
+  </si>
+  <si>
+    <t>November 2024</t>
+  </si>
+  <si>
+    <t>December 2024</t>
   </si>
 </sst>
 </file>
@@ -474,37 +474,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>14888.52</v>
+        <v>23946.79</v>
       </c>
       <c r="C2">
-        <v>27379.32</v>
+        <v>38000.25</v>
       </c>
       <c r="D2">
-        <v>20299.34</v>
+        <v>29777.47</v>
       </c>
       <c r="E2">
-        <v>24819.5</v>
-      </c>
-      <c r="F2">
-        <v>18894.48</v>
-      </c>
-      <c r="G2">
-        <v>17005.28</v>
-      </c>
-      <c r="H2">
-        <v>23443.38</v>
-      </c>
-      <c r="I2">
-        <v>14601.94</v>
-      </c>
-      <c r="J2">
-        <v>19625.17</v>
-      </c>
-      <c r="K2">
-        <v>12895.24</v>
-      </c>
-      <c r="L2">
-        <v>21685.31</v>
+        <v>252.55</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -512,37 +491,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>17784.62</v>
+        <v>14247.06</v>
       </c>
       <c r="C3">
-        <v>26486.53</v>
+        <v>24577.94</v>
       </c>
       <c r="D3">
-        <v>16581.79</v>
+        <v>14503.15</v>
       </c>
       <c r="E3">
-        <v>20093.13</v>
-      </c>
-      <c r="F3">
-        <v>8094.83</v>
-      </c>
-      <c r="G3">
-        <v>12039.55</v>
-      </c>
-      <c r="H3">
-        <v>12567.48</v>
-      </c>
-      <c r="I3">
-        <v>10108.42</v>
-      </c>
-      <c r="J3">
-        <v>15225.9</v>
-      </c>
-      <c r="K3">
-        <v>13628.38</v>
-      </c>
-      <c r="L3">
-        <v>10805.9</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -550,37 +508,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10281.97</v>
+        <v>13158.1</v>
       </c>
       <c r="C4">
-        <v>23566.01</v>
+        <v>13837.31</v>
       </c>
       <c r="D4">
-        <v>11406.17</v>
+        <v>15091.78</v>
       </c>
       <c r="E4">
-        <v>15615.67</v>
-      </c>
-      <c r="F4">
-        <v>18032.0</v>
-      </c>
-      <c r="G4">
-        <v>18197.54</v>
-      </c>
-      <c r="H4">
-        <v>15005.81</v>
-      </c>
-      <c r="I4">
-        <v>9754.63</v>
-      </c>
-      <c r="J4">
-        <v>14183.76</v>
-      </c>
-      <c r="K4">
-        <v>11373.27</v>
-      </c>
-      <c r="L4">
-        <v>7228.7</v>
+        <v>71.4</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -588,37 +525,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>15483.38</v>
+        <v>14057.65</v>
       </c>
       <c r="C5">
-        <v>26759.96</v>
+        <v>21966.88</v>
       </c>
       <c r="D5">
-        <v>17852.75</v>
+        <v>18512.01</v>
       </c>
       <c r="E5">
-        <v>22028.09</v>
-      </c>
-      <c r="F5">
-        <v>18154.85</v>
-      </c>
-      <c r="G5">
-        <v>18936.99</v>
-      </c>
-      <c r="H5">
-        <v>16399.25</v>
-      </c>
-      <c r="I5">
-        <v>15049.73</v>
-      </c>
-      <c r="J5">
-        <v>19370.68</v>
-      </c>
-      <c r="K5">
-        <v>14895.0</v>
-      </c>
-      <c r="L5">
-        <v>12901.95</v>
+        <v>77.52</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -626,37 +542,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7110.97</v>
+        <v>10130.05</v>
       </c>
       <c r="C6">
-        <v>13190.21</v>
+        <v>13869.15</v>
       </c>
       <c r="D6">
-        <v>3473.74</v>
+        <v>12724.67</v>
       </c>
       <c r="E6">
-        <v>11728.51</v>
-      </c>
-      <c r="F6">
-        <v>11386.77</v>
-      </c>
-      <c r="G6">
-        <v>11848.99</v>
-      </c>
-      <c r="H6">
-        <v>10730.01</v>
-      </c>
-      <c r="I6">
-        <v>9848.51</v>
-      </c>
-      <c r="J6">
-        <v>12250.91</v>
-      </c>
-      <c r="K6">
-        <v>10428.3</v>
-      </c>
-      <c r="L6">
-        <v>8272.31</v>
+        <v>179.52</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -664,37 +559,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10747.36</v>
+        <v>9575.21</v>
       </c>
       <c r="C7">
-        <v>16978.55</v>
+        <v>15078.69</v>
       </c>
       <c r="D7">
-        <v>11228.34</v>
-      </c>
-      <c r="E7">
-        <v>14855.39</v>
-      </c>
-      <c r="F7">
-        <v>12170.18</v>
-      </c>
-      <c r="G7">
-        <v>12503.96</v>
-      </c>
-      <c r="H7">
-        <v>8293.18</v>
-      </c>
-      <c r="I7">
-        <v>10439.91</v>
-      </c>
-      <c r="J7">
-        <v>11610.79</v>
-      </c>
-      <c r="K7">
-        <v>10844.91</v>
-      </c>
-      <c r="L7">
-        <v>8955.84</v>
+        <v>14467.49</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -702,57 +573,60 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>11790.98</v>
+        <v>11771.54</v>
       </c>
       <c r="C8">
-        <v>17335.67</v>
+        <v>12832.38</v>
       </c>
       <c r="D8">
-        <v>9610.25</v>
-      </c>
-      <c r="E8">
-        <v>7288.09</v>
-      </c>
-      <c r="F8">
-        <v>14696.73</v>
-      </c>
-      <c r="G8">
-        <v>14390.56</v>
-      </c>
-      <c r="H8">
-        <v>14665.29</v>
-      </c>
-      <c r="I8">
-        <v>12058.61</v>
-      </c>
-      <c r="J8">
-        <v>14421.22</v>
-      </c>
-      <c r="K8">
-        <v>13035.09</v>
-      </c>
-      <c r="L8">
-        <v>10075.15</v>
+        <v>13581.91</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>1561.22</v>
+      </c>
+      <c r="C9">
+        <v>110.76</v>
+      </c>
+      <c r="D9">
+        <v>14076.96</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>1272.09</v>
+      </c>
+      <c r="C10">
+        <v>44.88</v>
+      </c>
+      <c r="D10">
+        <v>12767.23</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>423.02</v>
+      </c>
+      <c r="C11">
+        <v>11767.22</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="C12">
+        <v>4006.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add func manage PA
</commit_message>
<xml_diff>
--- a/public/tmp/pivottotalwork.xlsx
+++ b/public/tmp/pivottotalwork.xlsx
@@ -53,37 +53,37 @@
     <t>พรชัย</t>
   </si>
   <si>
-    <t>February 2024</t>
-  </si>
-  <si>
-    <t>March 2024</t>
-  </si>
-  <si>
-    <t>April 2024</t>
-  </si>
-  <si>
-    <t>May 2024</t>
-  </si>
-  <si>
-    <t>June 2024</t>
-  </si>
-  <si>
-    <t>July 2024</t>
-  </si>
-  <si>
-    <t>August 2024</t>
-  </si>
-  <si>
-    <t>September 2024</t>
-  </si>
-  <si>
-    <t>October 2024</t>
-  </si>
-  <si>
-    <t>November 2024</t>
-  </si>
-  <si>
-    <t>December 2024</t>
+    <t>February 2023</t>
+  </si>
+  <si>
+    <t>March 2023</t>
+  </si>
+  <si>
+    <t>April 2023</t>
+  </si>
+  <si>
+    <t>May 2023</t>
+  </si>
+  <si>
+    <t>June 2023</t>
+  </si>
+  <si>
+    <t>July 2023</t>
+  </si>
+  <si>
+    <t>August 2023</t>
+  </si>
+  <si>
+    <t>September 2023</t>
+  </si>
+  <si>
+    <t>October 2023</t>
+  </si>
+  <si>
+    <t>November 2023</t>
+  </si>
+  <si>
+    <t>December 2023</t>
   </si>
 </sst>
 </file>
@@ -474,16 +474,37 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>23946.79</v>
+        <v>14888.52</v>
       </c>
       <c r="C2">
-        <v>38000.25</v>
+        <v>27379.32</v>
       </c>
       <c r="D2">
-        <v>29777.47</v>
+        <v>20299.34</v>
       </c>
       <c r="E2">
-        <v>252.55</v>
+        <v>24819.5</v>
+      </c>
+      <c r="F2">
+        <v>18894.48</v>
+      </c>
+      <c r="G2">
+        <v>17005.28</v>
+      </c>
+      <c r="H2">
+        <v>23443.38</v>
+      </c>
+      <c r="I2">
+        <v>14601.94</v>
+      </c>
+      <c r="J2">
+        <v>19625.17</v>
+      </c>
+      <c r="K2">
+        <v>12895.24</v>
+      </c>
+      <c r="L2">
+        <v>21685.31</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -491,16 +512,37 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14247.06</v>
+        <v>17784.62</v>
       </c>
       <c r="C3">
-        <v>24577.94</v>
+        <v>26486.53</v>
       </c>
       <c r="D3">
-        <v>14503.15</v>
+        <v>16581.79</v>
       </c>
       <c r="E3">
-        <v>112.6</v>
+        <v>20093.13</v>
+      </c>
+      <c r="F3">
+        <v>8094.83</v>
+      </c>
+      <c r="G3">
+        <v>12039.55</v>
+      </c>
+      <c r="H3">
+        <v>12567.48</v>
+      </c>
+      <c r="I3">
+        <v>10108.42</v>
+      </c>
+      <c r="J3">
+        <v>15225.9</v>
+      </c>
+      <c r="K3">
+        <v>13628.38</v>
+      </c>
+      <c r="L3">
+        <v>10805.9</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -508,16 +550,37 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>13158.1</v>
+        <v>10281.97</v>
       </c>
       <c r="C4">
-        <v>13837.31</v>
+        <v>23566.01</v>
       </c>
       <c r="D4">
-        <v>15091.78</v>
+        <v>11406.17</v>
       </c>
       <c r="E4">
-        <v>71.4</v>
+        <v>15615.67</v>
+      </c>
+      <c r="F4">
+        <v>18032.0</v>
+      </c>
+      <c r="G4">
+        <v>18197.54</v>
+      </c>
+      <c r="H4">
+        <v>15005.81</v>
+      </c>
+      <c r="I4">
+        <v>9754.63</v>
+      </c>
+      <c r="J4">
+        <v>14183.76</v>
+      </c>
+      <c r="K4">
+        <v>11373.27</v>
+      </c>
+      <c r="L4">
+        <v>7228.7</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -525,16 +588,37 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>14057.65</v>
+        <v>15483.38</v>
       </c>
       <c r="C5">
-        <v>21966.88</v>
+        <v>26759.96</v>
       </c>
       <c r="D5">
-        <v>18512.01</v>
+        <v>17852.75</v>
       </c>
       <c r="E5">
-        <v>77.52</v>
+        <v>22028.09</v>
+      </c>
+      <c r="F5">
+        <v>18154.85</v>
+      </c>
+      <c r="G5">
+        <v>18936.99</v>
+      </c>
+      <c r="H5">
+        <v>16399.25</v>
+      </c>
+      <c r="I5">
+        <v>15049.73</v>
+      </c>
+      <c r="J5">
+        <v>19370.68</v>
+      </c>
+      <c r="K5">
+        <v>14895.0</v>
+      </c>
+      <c r="L5">
+        <v>12901.95</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -542,16 +626,37 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10130.05</v>
+        <v>7110.97</v>
       </c>
       <c r="C6">
-        <v>13869.15</v>
+        <v>13190.21</v>
       </c>
       <c r="D6">
-        <v>12724.67</v>
+        <v>3473.74</v>
       </c>
       <c r="E6">
-        <v>179.52</v>
+        <v>11728.51</v>
+      </c>
+      <c r="F6">
+        <v>11386.77</v>
+      </c>
+      <c r="G6">
+        <v>11848.99</v>
+      </c>
+      <c r="H6">
+        <v>10730.01</v>
+      </c>
+      <c r="I6">
+        <v>9848.51</v>
+      </c>
+      <c r="J6">
+        <v>12250.91</v>
+      </c>
+      <c r="K6">
+        <v>10428.3</v>
+      </c>
+      <c r="L6">
+        <v>8272.31</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -559,13 +664,37 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>9575.21</v>
+        <v>10747.36</v>
       </c>
       <c r="C7">
-        <v>15078.69</v>
+        <v>16978.55</v>
       </c>
       <c r="D7">
-        <v>14467.49</v>
+        <v>11228.34</v>
+      </c>
+      <c r="E7">
+        <v>14855.39</v>
+      </c>
+      <c r="F7">
+        <v>12170.18</v>
+      </c>
+      <c r="G7">
+        <v>12503.96</v>
+      </c>
+      <c r="H7">
+        <v>8293.18</v>
+      </c>
+      <c r="I7">
+        <v>10439.91</v>
+      </c>
+      <c r="J7">
+        <v>11610.79</v>
+      </c>
+      <c r="K7">
+        <v>10844.91</v>
+      </c>
+      <c r="L7">
+        <v>8955.84</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -573,60 +702,57 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>11771.54</v>
+        <v>11790.98</v>
       </c>
       <c r="C8">
-        <v>12832.38</v>
+        <v>17335.67</v>
       </c>
       <c r="D8">
-        <v>13581.91</v>
+        <v>9610.25</v>
+      </c>
+      <c r="E8">
+        <v>7288.09</v>
+      </c>
+      <c r="F8">
+        <v>14696.73</v>
+      </c>
+      <c r="G8">
+        <v>14390.56</v>
+      </c>
+      <c r="H8">
+        <v>14665.29</v>
+      </c>
+      <c r="I8">
+        <v>12058.61</v>
+      </c>
+      <c r="J8">
+        <v>14421.22</v>
+      </c>
+      <c r="K8">
+        <v>13035.09</v>
+      </c>
+      <c r="L8">
+        <v>10075.15</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1561.22</v>
-      </c>
-      <c r="C9">
-        <v>110.76</v>
-      </c>
-      <c r="D9">
-        <v>14076.96</v>
-      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1272.09</v>
-      </c>
-      <c r="C10">
-        <v>44.88</v>
-      </c>
-      <c r="D10">
-        <v>12767.23</v>
-      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>423.02</v>
-      </c>
-      <c r="C11">
-        <v>11767.22</v>
-      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>11</v>
-      </c>
-      <c r="C12">
-        <v>4006.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>